<commit_message>
trabajo en ajax de granja
</commit_message>
<xml_diff>
--- a/_DOCs/webserviceV5.xlsx
+++ b/_DOCs/webserviceV5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Confe2\_DOCs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Confe2\_DOCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94883762-668A-4934-9281-B72D7E9C0742}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09C9280-CEEE-4FF3-991F-22FB7063755E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92E7474C-DBF9-422C-8A46-30790FC12D63}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14040" activeTab="3" xr2:uid="{92E7474C-DBF9-422C-8A46-30790FC12D63}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos WS" sheetId="1" r:id="rId1"/>
@@ -1152,7 +1152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{081A2071-6B82-4DF7-B58A-E6A87EDE448E}">
   <dimension ref="A5:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1765,11 +1765,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0627DF3-34FF-401C-8C73-99D44018DFCD}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="B4:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="12"/>
     <col min="2" max="2" width="24" style="11" customWidth="1"/>
@@ -1780,7 +1780,7 @@
     <col min="8" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>18</v>
       </c>
@@ -1788,7 +1788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>79</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>1</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>2</v>
       </c>
@@ -1852,7 +1852,7 @@
       </c>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>3</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>4</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>5</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>6</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>7</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>8</v>
       </c>
@@ -1975,7 +1975,7 @@
       <c r="F11" s="20"/>
       <c r="G11" s="18"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>9</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>10</v>
       </c>
@@ -2016,7 +2016,7 @@
       </c>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>11</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>12</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>13</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>14</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>15</v>
       </c>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>16</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>17</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>18</v>
       </c>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>19</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>20</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>21</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>22</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>23</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>24</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>25</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>26</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>27</v>
       </c>
@@ -2403,7 +2403,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>28</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>29</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>30</v>
       </c>
@@ -2470,7 +2470,7 @@
       </c>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>31</v>
       </c>
@@ -2491,7 +2491,7 @@
       </c>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>32</v>
       </c>
@@ -2512,7 +2512,7 @@
       </c>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>33</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Inicio imp Unidad 2
</commit_message>
<xml_diff>
--- a/_DOCs/webserviceV5.xlsx
+++ b/_DOCs/webserviceV5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Confe2\_DOCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5AFECB-ED77-4F42-B073-7C8318A5B13C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EA0638-4F0C-4DA4-BBA1-E38EFF12B8D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3636" yWindow="2076" windowWidth="17280" windowHeight="10884" activeTab="4" xr2:uid="{92E7474C-DBF9-422C-8A46-30790FC12D63}"/>
+    <workbookView xWindow="14916" yWindow="1308" windowWidth="20736" windowHeight="12360" activeTab="3" xr2:uid="{92E7474C-DBF9-422C-8A46-30790FC12D63}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos WS" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="163">
   <si>
     <t>-</t>
   </si>
@@ -298,9 +298,6 @@
     <t>Se debe contar con un perfil de super usuario que tenga acceso a las anteriores funcionalidades de manera global (no por grupo) . A parte de un módulo para hacer un CRUD de textos por juego</t>
   </si>
   <si>
-    <t>c02ropero2</t>
-  </si>
-  <si>
     <t>etiqueta</t>
   </si>
   <si>
@@ -406,27 +403,6 @@
     <t>j0101granja</t>
   </si>
   <si>
-    <t>j0202top10</t>
-  </si>
-  <si>
-    <t>r0202seleccion</t>
-  </si>
-  <si>
-    <t>j0203mandela</t>
-  </si>
-  <si>
-    <t>r0203bienaventuranzas</t>
-  </si>
-  <si>
-    <t>j0204flappybird</t>
-  </si>
-  <si>
-    <t>r0204exitofracaso</t>
-  </si>
-  <si>
-    <t>j0205acompanajesus</t>
-  </si>
-  <si>
     <t>ropero 1</t>
   </si>
   <si>
@@ -514,16 +490,40 @@
     <t>entero</t>
   </si>
   <si>
-    <t>c01ropero1</t>
-  </si>
-  <si>
-    <t>j01granja</t>
-  </si>
-  <si>
-    <t>r01emociones</t>
-  </si>
-  <si>
     <t>set_avance_juego</t>
+  </si>
+  <si>
+    <t>R02bienaventuranzas</t>
+  </si>
+  <si>
+    <t>J02flappybird</t>
+  </si>
+  <si>
+    <t>R02exitofracaso</t>
+  </si>
+  <si>
+    <t>J02acompanajesus</t>
+  </si>
+  <si>
+    <t>C01ropero1</t>
+  </si>
+  <si>
+    <t>R01emociones</t>
+  </si>
+  <si>
+    <t>J01granja</t>
+  </si>
+  <si>
+    <t>C02ropero2</t>
+  </si>
+  <si>
+    <t>J02top10</t>
+  </si>
+  <si>
+    <t>R02seleccion</t>
+  </si>
+  <si>
+    <t>J02mandela</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -669,6 +669,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -711,7 +717,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -791,6 +797,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1193,10 +1202,10 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C6" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -1208,7 +1217,7 @@
         <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H6" s="5">
         <v>7</v>
@@ -1216,7 +1225,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="26" t="s">
@@ -1241,7 +1250,7 @@
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>9</v>
@@ -1256,7 +1265,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>11</v>
@@ -1271,7 +1280,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>13</v>
@@ -1286,10 +1295,10 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>0</v>
@@ -1297,10 +1306,10 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C12" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -1310,7 +1319,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -1330,7 +1339,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="5"/>
@@ -1342,10 +1351,10 @@
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E17" s="30" t="s">
         <v>17</v>
@@ -1355,10 +1364,10 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C18" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E18" s="30"/>
       <c r="G18" s="1"/>
@@ -1366,7 +1375,7 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="5"/>
@@ -1403,34 +1412,34 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C34" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E34" s="28" t="s">
         <v>21</v>
@@ -1444,41 +1453,41 @@
     </row>
     <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B35" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C35" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E35" s="28" t="s">
         <v>12</v>
       </c>
       <c r="F35" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="G35" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="H35" t="s">
         <v>121</v>
-      </c>
-      <c r="H35" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E36" s="28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F36" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="G36" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E37" s="28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F37" t="b">
         <v>1</v>
@@ -1492,15 +1501,15 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C38" s="33"/>
       <c r="D38" s="34"/>
       <c r="E38" s="28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -1517,7 +1526,7 @@
       <c r="C39" s="33"/>
       <c r="D39" s="34"/>
       <c r="E39" s="28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F39" t="b">
         <v>0</v>
@@ -1563,10 +1572,10 @@
         <v>79</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1574,10 +1583,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E3" s="32" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1585,10 +1594,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E4" s="32" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1596,10 +1605,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="32" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1607,10 +1616,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1618,10 +1627,10 @@
         <v>5</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1629,10 +1638,10 @@
         <v>6</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1640,10 +1649,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="15.6" x14ac:dyDescent="0.3">
@@ -1651,7 +1660,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="32" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="E10" s="32"/>
     </row>
@@ -1660,7 +1669,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E11" s="32"/>
     </row>
@@ -1767,8 +1776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0627DF3-34FF-401C-8C73-99D44018DFCD}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1814,11 +1823,11 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+      <c r="A4" s="36">
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>34</v>
@@ -1834,11 +1843,11 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
+      <c r="A5" s="36">
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>33</v>
@@ -1855,11 +1864,11 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+      <c r="A6" s="36">
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>24</v>
@@ -1875,11 +1884,11 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
+      <c r="A7" s="36">
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>87</v>
+        <v>159</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>25</v>
@@ -1895,11 +1904,11 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
+      <c r="A8" s="36">
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>123</v>
+        <v>160</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>26</v>
@@ -1915,11 +1924,11 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="12">
+      <c r="A9" s="36">
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>124</v>
+        <v>161</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>27</v>
@@ -1938,11 +1947,11 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="12">
+      <c r="A10" s="36">
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>35</v>
@@ -1961,11 +1970,11 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
+      <c r="A11" s="36">
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>32</v>
@@ -1978,11 +1987,11 @@
       <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
+      <c r="A12" s="36">
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>28</v>
@@ -1998,11 +2007,11 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
+      <c r="A13" s="36">
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>36</v>
@@ -2019,11 +2028,11 @@
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
+      <c r="A14" s="36">
         <v>11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>37</v>
@@ -2046,7 +2055,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>39</v>
@@ -2069,7 +2078,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>41</v>
@@ -2092,7 +2101,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>43</v>
@@ -2115,7 +2124,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>45</v>
@@ -2136,7 +2145,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>46</v>
@@ -2159,7 +2168,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>47</v>
@@ -2182,7 +2191,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>49</v>
@@ -2203,7 +2212,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>50</v>
@@ -2226,7 +2235,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>52</v>
@@ -2249,7 +2258,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>54</v>
@@ -2272,7 +2281,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>56</v>
@@ -2295,7 +2304,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>58</v>
@@ -2318,7 +2327,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>59</v>
@@ -2341,7 +2350,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C28" s="21" t="s">
         <v>62</v>
@@ -2364,7 +2373,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>64</v>
@@ -2387,7 +2396,7 @@
         <v>27</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>66</v>
@@ -2410,7 +2419,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C31" s="23" t="s">
         <v>68</v>
@@ -2433,7 +2442,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>69</v>
@@ -2456,7 +2465,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>71</v>
@@ -2477,7 +2486,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>73</v>
@@ -2498,7 +2507,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>74</v>
@@ -2519,7 +2528,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>75</v>
@@ -2539,7 +2548,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>76</v>
@@ -2564,7 +2573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A728DB-C7AD-4923-B39C-73D7C99CB88B}">
   <dimension ref="E3:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
integracion juegos - menu fase 1
se agregan los botones y se envia parametro a sub menu
</commit_message>
<xml_diff>
--- a/_DOCs/webserviceV5.xlsx
+++ b/_DOCs/webserviceV5.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Confe2\_DOCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EA0638-4F0C-4DA4-BBA1-E38EFF12B8D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AD28E0-1592-4E36-A05A-9F66397DB322}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14916" yWindow="1308" windowWidth="20736" windowHeight="12360" activeTab="3" xr2:uid="{92E7474C-DBF9-422C-8A46-30790FC12D63}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{92E7474C-DBF9-422C-8A46-30790FC12D63}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos WS" sheetId="1" r:id="rId1"/>
     <sheet name="Trajes" sheetId="4" r:id="rId2"/>
     <sheet name="Administrador" sheetId="3" r:id="rId3"/>
     <sheet name="Tabla juegos" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="Tiempos" sheetId="5" r:id="rId5"/>
+    <sheet name="Objetos por unidad" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="172">
   <si>
     <t>-</t>
   </si>
@@ -524,6 +525,33 @@
   </si>
   <si>
     <t>J02mandela</t>
+  </si>
+  <si>
+    <t># unidad</t>
+  </si>
+  <si>
+    <t>objeto</t>
+  </si>
+  <si>
+    <t>sandalias</t>
+  </si>
+  <si>
+    <t>estrella</t>
+  </si>
+  <si>
+    <t>consultar con Pedro (se integra dentro del top 10)</t>
+  </si>
+  <si>
+    <t>cruz</t>
+  </si>
+  <si>
+    <t>paloma</t>
+  </si>
+  <si>
+    <t>agua y aceite</t>
+  </si>
+  <si>
+    <t>fuego</t>
   </si>
 </sst>
 </file>
@@ -789,6 +817,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -797,9 +828,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1503,11 +1531,11 @@
       <c r="A38" t="s">
         <v>131</v>
       </c>
-      <c r="B38" s="33" t="s">
+      <c r="B38" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="C38" s="33"/>
-      <c r="D38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="35"/>
       <c r="E38" s="28" t="s">
         <v>89</v>
       </c>
@@ -1522,9 +1550,9 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="34"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="35"/>
       <c r="E39" s="28" t="s">
         <v>91</v>
       </c>
@@ -1690,16 +1718,16 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -1722,45 +1750,45 @@
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1776,8 +1804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0627DF3-34FF-401C-8C73-99D44018DFCD}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1823,7 +1851,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="36">
+      <c r="A4" s="33">
         <v>1</v>
       </c>
       <c r="B4" s="11" t="s">
@@ -1843,7 +1871,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="36">
+      <c r="A5" s="33">
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
@@ -1864,7 +1892,7 @@
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="36">
+      <c r="A6" s="33">
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -1884,7 +1912,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="36">
+      <c r="A7" s="33">
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -1904,7 +1932,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="36">
+      <c r="A8" s="33">
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -1924,7 +1952,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="36">
+      <c r="A9" s="33">
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -1943,11 +1971,11 @@
         <v>3</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>77</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="36">
+      <c r="A10" s="33">
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -1970,7 +1998,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="36">
+      <c r="A11" s="33">
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -1987,7 +2015,7 @@
       <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="36">
+      <c r="A12" s="33">
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -2007,7 +2035,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="36">
+      <c r="A13" s="33">
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -2028,7 +2056,7 @@
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="36">
+      <c r="A14" s="33">
         <v>11</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -2573,7 +2601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A728DB-C7AD-4923-B39C-73D7C99CB88B}">
   <dimension ref="E3:I38"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
@@ -2932,4 +2960,75 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69AD94DF-86D8-4670-B83B-402C2A6E3983}">
+  <dimension ref="B2:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
imp objetos y avance en menu
</commit_message>
<xml_diff>
--- a/_DOCs/webserviceV5.xlsx
+++ b/_DOCs/webserviceV5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Confe2\_DOCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AD28E0-1592-4E36-A05A-9F66397DB322}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765C4808-2951-4500-8346-A958E78E2817}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{92E7474C-DBF9-422C-8A46-30790FC12D63}"/>
   </bookViews>
@@ -533,25 +533,25 @@
     <t>objeto</t>
   </si>
   <si>
-    <t>sandalias</t>
-  </si>
-  <si>
-    <t>estrella</t>
-  </si>
-  <si>
     <t>consultar con Pedro (se integra dentro del top 10)</t>
   </si>
   <si>
-    <t>cruz</t>
-  </si>
-  <si>
-    <t>paloma</t>
-  </si>
-  <si>
-    <t>agua y aceite</t>
-  </si>
-  <si>
-    <t>fuego</t>
+    <t>Sandalias</t>
+  </si>
+  <si>
+    <t>Estrella</t>
+  </si>
+  <si>
+    <t>Cruz</t>
+  </si>
+  <si>
+    <t>Paloma</t>
+  </si>
+  <si>
+    <t>AguaAceite</t>
+  </si>
+  <si>
+    <t>Fuego</t>
   </si>
 </sst>
 </file>
@@ -1971,7 +1971,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2967,7 +2967,7 @@
   <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2985,7 +2985,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -2993,7 +2993,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">

</xml_diff>